<commit_message>
Update to version 1.0.0
</commit_message>
<xml_diff>
--- a/Test/HeCalc_Input_withCorrelation_Example.xlsx
+++ b/Test/HeCalc_Input_withCorrelation_Example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pemar\Documents\FlowersResearch\Lab_procedures\Data_Processing_Program\HeCalc_git\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C11D25F-5A31-4CA7-937F-7E64C684A3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500046AB-6308-4EFA-A813-BCE70593C23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,10 +558,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="5">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
Update to version 1.0.1
</commit_message>
<xml_diff>
--- a/Test/HeCalc_Input_withCorrelation_Example.xlsx
+++ b/Test/HeCalc_Input_withCorrelation_Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pemar\Documents\FlowersResearch\Lab_procedures\Data_Processing_Program\HeCalc_git\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500046AB-6308-4EFA-A813-BCE70593C23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B618CA9-6853-4D4A-AFDE-7CAF8E9AC2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -164,7 +164,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z245"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,160 +556,160 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2">
         <v>0.1</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2">
         <v>1E-3</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2">
         <v>0.05</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2">
         <v>0.05</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2">
         <v>0.05</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2">
         <v>0.7</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2">
         <v>0.05</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2">
         <v>0.7</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2">
         <v>0.05</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2">
         <v>0.7</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2">
         <v>0.05</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2">
         <v>0.7</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="Q2">
         <v>0.05</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2">
         <v>0.1</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2">
         <v>0.1</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2">
         <v>0.1</v>
       </c>
-      <c r="U2" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="V2" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="W2" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="X2" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="Z2" s="5">
-        <v>0.9</v>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3">
         <v>0.1</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3">
         <v>0.05</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3">
         <v>0.05</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3">
         <v>0.05</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3">
         <v>0.7</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3">
         <v>0.05</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3">
         <v>0.7</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3">
         <v>0.05</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3">
         <v>0.7</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3">
         <v>0.05</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3">
         <v>0.7</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="Q3">
         <v>0.05</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3">
         <v>0.1</v>
       </c>
-      <c r="S3" s="5">
+      <c r="S3">
         <v>0.1</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3">
         <v>0.1</v>
       </c>
-      <c r="U3" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="V3" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="W3" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="X3" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="Z3" s="5">
-        <v>0.9</v>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>